<commit_message>
DOMA-3092 update xlsx contact import templates
</commit_message>
<xml_diff>
--- a/apps/condo/public/contact-import-example.xlsx
+++ b/apps/condo/public/contact-import-example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Address</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Unit Type</t>
   </si>
   <si>
     <t xml:space="preserve"> г Арамиль, ул Гарнизон, д 19Б</t>
@@ -300,13 +303,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -405,10 +402,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -663,13 +660,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -982,10 +973,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1267,27 +1258,27 @@
         <v>4</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">

</xml_diff>

<commit_message>
DOMA-4085 update excel template
</commit_message>
<xml_diff>
--- a/apps/condo/public/contact-import-example.xlsx
+++ b/apps/condo/public/contact-import-example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Address</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Role</t>
   </si>
   <si>
     <t xml:space="preserve"> г Арамиль, ул Гарнизон, д 19Б</t>
@@ -51,6 +54,9 @@
       </rPr>
       <t>test@example.com</t>
     </r>
+  </si>
+  <si>
+    <t>Собственник</t>
   </si>
 </sst>
 </file>
@@ -1227,7 +1233,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1238,8 +1244,8 @@
     <col min="3" max="3" width="17.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.6719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6719" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="7" width="17.6719" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1261,25 +1267,31 @@
       <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
@@ -1289,6 +1301,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" s="6"/>
@@ -1297,6 +1310,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" s="6"/>
@@ -1305,6 +1319,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" s="6"/>
@@ -1313,6 +1328,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" s="6"/>
@@ -1321,6 +1337,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="6"/>
@@ -1329,6 +1346,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="6"/>
@@ -1337,6 +1355,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="6"/>
@@ -1345,6 +1364,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" s="6"/>
@@ -1353,6 +1373,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" s="6"/>
@@ -1361,6 +1382,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" s="6"/>
@@ -1369,6 +1391,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" s="6"/>
@@ -1377,6 +1400,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" s="6"/>
@@ -1385,6 +1409,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" s="6"/>
@@ -1393,6 +1418,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" s="6"/>
@@ -1401,6 +1427,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" s="6"/>
@@ -1409,6 +1436,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" s="6"/>
@@ -1417,6 +1445,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" s="6"/>
@@ -1425,6 +1454,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" s="6"/>
@@ -1433,6 +1463,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" s="6"/>
@@ -1441,6 +1472,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="6"/>
@@ -1449,6 +1481,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" s="6"/>
@@ -1457,6 +1490,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" s="6"/>
@@ -1465,6 +1499,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" s="6"/>
@@ -1473,6 +1508,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" s="6"/>
@@ -1481,6 +1517,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" s="6"/>
@@ -1489,6 +1526,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" s="6"/>
@@ -1497,6 +1535,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" s="6"/>
@@ -1505,6 +1544,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" s="6"/>
@@ -1513,6 +1553,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" s="6"/>
@@ -1521,6 +1562,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" s="6"/>
@@ -1529,6 +1571,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" s="6"/>
@@ -1537,6 +1580,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" s="6"/>
@@ -1545,6 +1589,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" s="6"/>
@@ -1553,6 +1598,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
     </row>
     <row r="37" ht="15.35" customHeight="1">
       <c r="A37" s="6"/>
@@ -1561,6 +1607,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" s="6"/>
@@ -1569,6 +1616,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
     </row>
     <row r="39" ht="15.35" customHeight="1">
       <c r="A39" s="6"/>
@@ -1577,6 +1625,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
     </row>
     <row r="40" ht="15.35" customHeight="1">
       <c r="A40" s="6"/>
@@ -1585,6 +1634,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
     </row>
     <row r="41" ht="15.35" customHeight="1">
       <c r="A41" s="6"/>
@@ -1593,6 +1643,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
     </row>
     <row r="42" ht="15.35" customHeight="1">
       <c r="A42" s="6"/>
@@ -1601,6 +1652,7 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
     </row>
     <row r="43" ht="15.35" customHeight="1">
       <c r="A43" s="6"/>
@@ -1609,6 +1661,7 @@
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
     </row>
     <row r="44" ht="15.35" customHeight="1">
       <c r="A44" s="6"/>
@@ -1617,6 +1670,7 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
     </row>
     <row r="45" ht="15.35" customHeight="1">
       <c r="A45" s="6"/>
@@ -1625,6 +1679,7 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
     </row>
     <row r="46" ht="15.35" customHeight="1">
       <c r="A46" s="6"/>
@@ -1633,6 +1688,7 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
     </row>
     <row r="47" ht="15.35" customHeight="1">
       <c r="A47" s="6"/>
@@ -1641,6 +1697,7 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
     </row>
     <row r="48" ht="15.35" customHeight="1">
       <c r="A48" s="6"/>
@@ -1649,6 +1706,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
     </row>
     <row r="49" ht="15.35" customHeight="1">
       <c r="A49" s="6"/>
@@ -1657,6 +1715,7 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
     </row>
     <row r="50" ht="15.35" customHeight="1">
       <c r="A50" s="6"/>
@@ -1665,6 +1724,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>